<commit_message>
Tested a prototypical german model.
</commit_message>
<xml_diff>
--- a/Models/transformer_to_transformer_architecture/analysis.xlsx
+++ b/Models/transformer_to_transformer_architecture/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Models\transformer_to_transformer_architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF33ECD-D841-4301-A1E8-A0B8AE24E23A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B60B7B-C124-4CAA-8B9E-03CCE3C04FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
+    <workbookView xWindow="5580" yWindow="165" windowWidth="21405" windowHeight="15435" xr2:uid="{F5E92E8A-8577-4490-95F3-1F336C079EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -819,9 +819,15 @@
       <c r="G6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="14">
+        <v>0.13772999999999999</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.23014999999999999</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0.15997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>